<commit_message>
update master assessment with version
</commit_message>
<xml_diff>
--- a/TF.Module/DatabaseUpdate/TF.xlsx
+++ b/TF.Module/DatabaseUpdate/TF.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\TF\TF.Module\DatabaseUpdate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9060D868-EE18-49DC-956E-D4288EE3FC51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{241746F6-4E7C-4CEF-89F7-363747E8E7AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{802C2848-CF66-C14E-8907-0699AA2D98C9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{802C2848-CF66-C14E-8907-0699AA2D98C9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Mechanisms" sheetId="1" r:id="rId1"/>
-    <sheet name="Metrics" sheetId="3" r:id="rId2"/>
+    <sheet name="Main" sheetId="4" r:id="rId1"/>
+    <sheet name="Mechanisms" sheetId="1" r:id="rId2"/>
+    <sheet name="Metrics" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Mechanisms!$A$1:$R$49</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Metrics!$A$1:$M$476</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Mechanisms!$A$1:$R$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Metrics!$A$1:$M$476</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3160" uniqueCount="1512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3161" uniqueCount="1513">
   <si>
     <t>Code</t>
   </si>
@@ -4626,6 +4627,9 @@
   </si>
   <si>
     <t>S.FAM.D3</t>
+  </si>
+  <si>
+    <t>Created On:</t>
   </si>
 </sst>
 </file>
@@ -4684,13 +4688,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5153,11 +5158,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77CA0E7B-372D-4E60-B459-EF21C7B1F8C2}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.625" customWidth="1"/>
+    <col min="2" max="2" width="10.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1512</v>
+      </c>
+      <c r="B1" s="4">
+        <v>45016</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C81902B2-D680-544E-8D15-2C5362A2301D}">
   <dimension ref="A1:R49"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="L52" sqref="L52"/>
     </sheetView>
@@ -6967,14 +6999,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D9E030-DC72-1242-8D47-8AB6D70A0A27}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:P476"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C151" sqref="C151"/>
+      <selection pane="bottomLeft" activeCell="E152" sqref="E152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update date on seeds
</commit_message>
<xml_diff>
--- a/TF.Module/DatabaseUpdate/TF.xlsx
+++ b/TF.Module/DatabaseUpdate/TF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mirko\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D720E68-CE86-4C3F-A827-A5D6B5C21AAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CF893B-5561-4E53-9B98-BC98857F7E04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2955" yWindow="1845" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{802C2848-CF66-C14E-8907-0699AA2D98C9}"/>
+    <workbookView xWindow="2955" yWindow="1845" windowWidth="21600" windowHeight="11295" xr2:uid="{802C2848-CF66-C14E-8907-0699AA2D98C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="6" r:id="rId1"/>
@@ -7603,8 +7603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F94436C4-BB3B-4EA9-99CE-53C39ECBC708}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7618,7 +7618,7 @@
         <v>1530</v>
       </c>
       <c r="B1" s="4">
-        <v>45019</v>
+        <v>45030</v>
       </c>
     </row>
   </sheetData>
@@ -9448,7 +9448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D9E030-DC72-1242-8D47-8AB6D70A0A27}">
   <dimension ref="A1:U381"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I21" sqref="I21"/>
     </sheetView>
@@ -48421,11 +48421,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="dd7aa49a-064a-456f-962d-fecf52e7bc47" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -48646,27 +48647,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="dd7aa49a-064a-456f-962d-fecf52e7bc47" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52C0DD01-18EB-4042-863E-ABF196DEC34A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C333E94-3822-4FD9-AC3E-39D678C7030D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="dd7aa49a-064a-456f-962d-fecf52e7bc47"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="ad6c24f1-153f-4463-b202-cc8a5fbc0802"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -48691,9 +48682,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C333E94-3822-4FD9-AC3E-39D678C7030D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52C0DD01-18EB-4042-863E-ABF196DEC34A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="dd7aa49a-064a-456f-962d-fecf52e7bc47"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="ad6c24f1-153f-4463-b202-cc8a5fbc0802"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>